<commit_message>
Formatting submissions for airtable
</commit_message>
<xml_diff>
--- a/aicsairtable/data/LaserPower_dashboard_headers.xlsx
+++ b/aicsairtable/data/LaserPower_dashboard_headers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\aics\microscopy\brian_whitney\repos\aicsairtable\aicsairtable\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\aics\microscopy\brian_whitney\repos\aicsairtable\aicsairtable\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FE726C-7453-4195-AA37-60A2A7EF26E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD009A43-1280-455D-81E9-AF9BF529B4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23265" yWindow="2595" windowWidth="21600" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,15 +28,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Wavelength</t>
-  </si>
-  <si>
-    <t>Laser Power at 100%</t>
-  </si>
-  <si>
-    <t>Expiramental (% laser power)</t>
-  </si>
-  <si>
     <t>R^2</t>
   </si>
   <si>
@@ -44,6 +35,15 @@
   </si>
   <si>
     <t>Current</t>
+  </si>
+  <si>
+    <t>Laser Power at 100% (uW)</t>
+  </si>
+  <si>
+    <t>Wavelength (nm)</t>
+  </si>
+  <si>
+    <t>Experimental Laser Power (% laser power)</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:H197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,22 +429,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>